<commit_message>
finalisation du projet et de l'interface graphique
</commit_message>
<xml_diff>
--- a/data/CartesReduction.xlsx
+++ b/data/CartesReduction.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,34 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C00005</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>000002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C00006</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
correction et retrait des donnees non conformes a la consigne
</commit_message>
<xml_diff>
--- a/data/CartesReduction.xlsx
+++ b/data/CartesReduction.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,10 +464,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>000002</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -476,6 +474,21 @@
       </c>
       <c r="C3" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>000003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C00009</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>